<commit_message>
added stop condition, beginning conditions
</commit_message>
<xml_diff>
--- a/flowshop_problem/stats/algorithms_stats.xlsx
+++ b/flowshop_problem/stats/algorithms_stats.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikuba\PycharmProjects\SPD\flowshop_problem\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20551593-636E-4DC3-87A5-D1C184DFEDF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E19365-172E-4431-A63E-E560741A9569}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1428" windowWidth="23256" windowHeight="12576" xr2:uid="{CB874C67-1AA7-491E-8DC2-147ABB7F12DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CB874C67-1AA7-491E-8DC2-147ABB7F12DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Podsumowanie" sheetId="2" r:id="rId1"/>
     <sheet name="Dane" sheetId="1" r:id="rId2"/>
+    <sheet name="tabu search wnioski" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="19" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
   <si>
     <t>Algorytm</t>
   </si>
@@ -78,6 +79,66 @@
   <si>
     <t>Suma z t [ms]</t>
   </si>
+  <si>
+    <t>Suma z Cmax  [średnia]</t>
+  </si>
+  <si>
+    <t>tabu search 80 iteracji, zmodyfikowany random swap + johnson na start</t>
+  </si>
+  <si>
+    <t>tabu search 50 iteracji, zmodyfikowany random swap + johnson na start</t>
+  </si>
+  <si>
+    <t>tabu search 20 iteracji, zmodyfikowany random swap + johnson na start</t>
+  </si>
+  <si>
+    <t>Iteracje</t>
+  </si>
+  <si>
+    <t>Wniosek</t>
+  </si>
+  <si>
+    <t>tabu search 30 iteracji, zmodyfikowany random swap + johnson na start</t>
+  </si>
+  <si>
+    <t>Zwiększanie liczby iteracji poprawia wyniki, jednak po przekroczeniu pewnej granicy zyski jakie mamy w rezultatach nie kompensują znacznego pogorszenia czasu</t>
+  </si>
+  <si>
+    <t>Składowa</t>
+  </si>
+  <si>
+    <t>tabu search 200 iteracji, zmodyfikowany random swap + johnson na start</t>
+  </si>
+  <si>
+    <t>Dla małej liczby zadań (20) możemy zwiększyć liczbe iteracji (np. do 200,300), wtedy czas nie będzie aż tak duży (rzędu kilku sekund), a wyniki są lepsze od NEHa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Im więcej iteracji, tym większy czas trwania, zmiana czasu jest liniowa</t>
+  </si>
+  <si>
+    <t>Dla większej liczby zadań możemy zmniejszyć liczbę iteracji w ten sposób uzyskamy czasy wykonywania lepsze od NEHa a wyniki podobne</t>
+  </si>
+  <si>
+    <t>warunki początkowe</t>
+  </si>
+  <si>
+    <t>Dla dużej liczby iteracji wejście tabu searcha ma mniejsze znaczenie, ale dla mniejszej liczby iteracji (np. do 150) algorytm daje lepsze wyniki z johnsonem na starcie</t>
+  </si>
+  <si>
+    <t>Dla małej liczby zadań (20/50) można na początek dać NEHa, ponieważ działa on na mniejszej liczbie zadań dość szybko - wyniki są lepsze, a dla dużej liczby zadań lepiej dać na start johnsona ze względu na czas wykonania</t>
+  </si>
+  <si>
+    <t>kryterium stopu</t>
+  </si>
+  <si>
+    <t>liczba iteracji - opisana wyżej</t>
+  </si>
+  <si>
+    <t>Gdy przyjmiemy czas potrzebny na policzenia NEHa przy dużej liczbie zadań, wtedy otrzymujemy lepsze wyniki w algorytmie metaheurystycznym</t>
+  </si>
+  <si>
+    <t>Czas trwania algorytmu - np. algorytm ma zakończyć pracę po 10 sekundach - to kryterium może sprawdzać się dla bardzo dużej liczby zadań, gdzie potrzebujemy jakieś rozwiązanie, a nie możemy liczyć w nieskończoność</t>
+  </si>
 </sst>
 </file>
 
@@ -86,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +208,24 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -166,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -378,88 +457,151 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Dane wyjściowe" xfId="1" builtinId="21"/>
     <cellStyle name="Komórka zaznaczona" xfId="2" builtinId="23"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="162">
+  <dxfs count="92">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -625,6 +767,21 @@
       </border>
     </dxf>
     <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
@@ -789,6 +946,21 @@
       </border>
     </dxf>
     <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
@@ -953,824 +1125,34 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <border>
@@ -2473,6 +1855,62 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -2489,7 +1927,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Suma</c:v>
+                  <c:v>Suma z t [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2506,9 +1944,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Podsumowanie!$A$5:$A$10</c:f>
+              <c:f>Podsumowanie!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Johnson N maszynowy</c:v>
                 </c:pt>
@@ -2527,15 +1965,18 @@
                 <c:pt idx="5">
                   <c:v>NEH rozszerzony 4</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>tabu search 200 iteracji, zmodyfikowany random swap + johnson na start</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Podsumowanie!$B$5:$B$10</c:f>
+              <c:f>Podsumowanie!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.405</c:v>
                 </c:pt>
@@ -2554,12 +1995,104 @@
                 <c:pt idx="5">
                   <c:v>251.887</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>1765</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-D588-45A6-8549-D6B7BF3B4155}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Podsumowanie!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Suma z Cmax  [średnia]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Podsumowanie!$A$5:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Johnson N maszynowy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NEH</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NEH rozszerzony 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NEH rozszerzony 2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NEH rozszerzony 3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>NEH rozszerzony 4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tabu search 200 iteracji, zmodyfikowany random swap + johnson na start</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Podsumowanie!$C$5:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1777</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1578</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1562</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D778-4DD4-B8FA-C61DBA1ED8A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3331,15 +2864,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>253477</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>219578</xdr:rowOff>
+      <xdr:colOff>612065</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>17874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>475130</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>235323</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>233082</xdr:rowOff>
+      <xdr:rowOff>134472</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3368,40 +2901,49 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kuba Kędzierski" refreshedDate="44292.563955671299" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="48" xr:uid="{450CD30C-5766-4FCA-AD83-B8F9F9C3F703}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kuba Kędzierski" refreshedDate="44300.693982638892" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="55" xr:uid="{11B2C4DB-0C22-45FA-8AB2-B400B190B13A}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="E6:I54" sheet="Dane"/>
+    <worksheetSource ref="E6:I214" sheet="Dane"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Algorytm" numFmtId="0">
-      <sharedItems count="6">
+      <sharedItems containsBlank="1" count="13">
         <s v="Johnson N maszynowy"/>
         <s v="NEH"/>
         <s v="NEH rozszerzony 1"/>
         <s v="NEH rozszerzony 2"/>
         <s v="NEH rozszerzony 3"/>
         <s v="NEH rozszerzony 4"/>
+        <s v="tabu search 80 iteracji, zmodyfikowany random swap + johnson na start"/>
+        <s v="tabu search 50 iteracji, zmodyfikowany random swap + johnson na start"/>
+        <s v="tabu search 20 iteracji, zmodyfikowany random swap + johnson na start"/>
+        <s v="tabu search 30 iteracji, zmodyfikowany random swap + johnson na start"/>
+        <s v="tabu search 200 iteracji, zmodyfikowany random swap + johnson na start"/>
+        <m/>
+        <s v="tabu search 200 iteracji" u="1"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Cmax  [średnia]" numFmtId="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1248.8" maxValue="11632"/>
+    <cacheField name="Cmax  [średnia]" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1248.8" maxValue="11632"/>
     </cacheField>
-    <cacheField name="t [ms]" numFmtId="164">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.004" maxValue="145707"/>
+    <cacheField name="t [ms]" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.004" maxValue="145707"/>
     </cacheField>
     <cacheField name="liczba zadań" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="20" maxValue="200" count="4">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="20" maxValue="200" count="5">
         <n v="20"/>
         <n v="50"/>
         <n v="100"/>
         <n v="200"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="liczba maszyn" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="5" maxValue="20" count="3">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="5" maxValue="20" count="4">
         <n v="5"/>
         <n v="10"/>
         <n v="20"/>
+        <m/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -3414,7 +2956,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="48">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="55">
   <r>
     <x v="0"/>
     <n v="1382.8"/>
@@ -3751,26 +3293,92 @@
     <x v="3"/>
     <x v="0"/>
   </r>
+  <r>
+    <x v="6"/>
+    <n v="2297"/>
+    <n v="953.4"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2307"/>
+    <n v="588.6"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="2326"/>
+    <n v="356.8"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3925"/>
+    <n v="10703"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="4018"/>
+    <n v="3839"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="1556"/>
+    <n v="1765"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="3"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F4E76F6C-28FD-43B9-94D8-6AC06D215407}" name="Tabela przestawna1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Algorytm  ">
-  <location ref="A4:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF3F0DB-C94A-4912-8435-A3E0BD722A82}" name="Tabela przestawna1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Algorytm  ">
+  <location ref="A4:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
-      <items count="7">
+      <items count="14">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item m="1" x="12"/>
+        <item x="11"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisPage" showAll="0">
       <items count="5">
         <item x="0"/>
@@ -3780,19 +3388,11 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -3811,99 +3411,154 @@
     <i>
       <x v="5"/>
     </i>
+    <i>
+      <x v="12"/>
+    </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
   </colItems>
   <pageFields count="2">
     <pageField fld="3" item="0" hier="-1"/>
     <pageField fld="4" item="1" hier="-1"/>
   </pageFields>
-  <dataFields count="1">
+  <dataFields count="2">
     <dataField name="Suma z t [ms]" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Suma z Cmax  [średnia]" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="18">
-    <format dxfId="161">
+  <formats count="23">
+    <format dxfId="91">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="160">
+    <format dxfId="90">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="159">
+    <format dxfId="89">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="158">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="157">
+    <format dxfId="87">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="156">
+    <format dxfId="86">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="155">
+    <format dxfId="85">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="154">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="153">
+    <format dxfId="83">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="152">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="151">
+    <format dxfId="81">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="150">
+    <format dxfId="80">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="149">
+    <format dxfId="79">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="148">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="147">
+    <format dxfId="77">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="146">
+    <format dxfId="76">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="145">
+    <format dxfId="75">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="144">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
+    <format dxfId="73">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="72">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="71">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="70">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="7">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
   </formats>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="0" format="8" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -4220,180 +3875,202 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C1B5508-3774-44D2-93BC-D3D6801778E0}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="27" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="24">
         <v>20</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="24">
         <v>10</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="25"/>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C4"/>
+      <c r="C4" s="28" t="s">
+        <v>13</v>
+      </c>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="29">
         <v>1.405</v>
       </c>
-      <c r="C5"/>
+      <c r="C5" s="29">
+        <v>1777</v>
+      </c>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="29">
         <v>85.587999999999994</v>
       </c>
-      <c r="C6"/>
+      <c r="C6" s="29">
+        <v>1583</v>
+      </c>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="29">
         <v>176.608</v>
       </c>
-      <c r="C7"/>
+      <c r="C7" s="29">
+        <v>1579</v>
+      </c>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="29">
         <v>169.8</v>
       </c>
-      <c r="C8"/>
+      <c r="C8" s="29">
+        <v>1575</v>
+      </c>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="29">
         <v>170.107</v>
       </c>
-      <c r="C9"/>
+      <c r="C9" s="29">
+        <v>1578</v>
+      </c>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="29">
         <v>251.887</v>
       </c>
-      <c r="C10"/>
+      <c r="C10" s="29">
+        <v>1562</v>
+      </c>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
+    <row r="11" spans="1:7" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="29">
+        <v>1765</v>
+      </c>
+      <c r="C11" s="29">
+        <v>1556</v>
+      </c>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12"/>
-    </row>
-    <row r="13" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12"/>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13"/>
+      <c r="C13"/>
     </row>
     <row r="14" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14"/>
-      <c r="B14"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
     </row>
     <row r="15" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15"/>
-      <c r="B15"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
     </row>
     <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16"/>
-      <c r="B16"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
     </row>
     <row r="17" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17"/>
+      <c r="A17" s="30"/>
     </row>
     <row r="18" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18"/>
+      <c r="A18" s="30"/>
     </row>
     <row r="19" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19"/>
+      <c r="A19" s="30"/>
     </row>
     <row r="20" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20"/>
+      <c r="A20" s="30"/>
     </row>
     <row r="21" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21"/>
+      <c r="A21" s="30"/>
     </row>
     <row r="22" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22"/>
+      <c r="A22" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4404,869 +4081,1011 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{929F22A8-E983-4847-84A3-FE2FC09A0A6D}">
-  <dimension ref="E4:I54"/>
+  <dimension ref="E4:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" topLeftCell="C48" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="25.85546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="17" style="11" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17" style="4" customWidth="1"/>
     <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="5:9" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="5:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="8">
         <f>1.3828*10^3</f>
         <v>1382.8</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="9">
         <v>1.004</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="10">
         <v>20</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="11">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="5:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="13">
         <v>1261.0999999999999</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="14">
         <v>41.79</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="15">
         <v>20</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="5:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="13">
         <v>1248.8</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="14">
         <v>86.29</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="15">
         <v>20</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="5:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="13">
         <v>1258.8</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="14">
         <v>83.11</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="15">
         <v>20</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="5:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="13">
         <v>1255.3</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="14">
         <v>83.6</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="15">
         <v>20</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="5:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="18">
         <v>1255.4000000000001</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="19">
         <v>121.19</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="20">
         <v>20</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="8">
         <v>1777</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="9">
         <v>1.405</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="10">
         <v>20</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="13">
         <v>1583</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="14">
         <v>85.587999999999994</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="15">
         <v>20</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="13">
         <v>1579</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="14">
         <v>176.608</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="15">
         <v>20</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="13">
         <v>1575</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="14">
         <v>169.8</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="15">
         <v>20</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="13">
         <v>1578</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="14">
         <v>170.107</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="15">
         <v>20</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="18">
         <v>1562</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="19">
         <v>251.887</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H18" s="20">
         <v>20</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="21">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="8">
         <v>2590</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="9">
         <v>1.9</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H19" s="10">
         <v>20</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="11">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="13">
         <v>2318.6999999999998</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="14">
         <v>167.28290000000001</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="15">
         <v>20</v>
       </c>
-      <c r="I20" s="23">
+      <c r="I20" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="13">
         <v>2322</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="14">
         <v>346.69900000000001</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="15">
         <v>20</v>
       </c>
-      <c r="I21" s="23">
+      <c r="I21" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="13">
         <v>2312.1</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="14">
         <v>328.10599999999999</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="15">
         <v>20</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="13">
         <v>2320.1</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="14">
         <v>342.99299999999999</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="15">
         <v>20</v>
       </c>
-      <c r="I23" s="23">
+      <c r="I23" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="18">
         <v>2300.3000000000002</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="19">
         <v>484.149</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="20">
         <v>20</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="21">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="8">
         <v>2967</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G25" s="9">
         <v>2.3010000000000002</v>
       </c>
-      <c r="H25" s="17">
+      <c r="H25" s="10">
         <v>50</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I25" s="11">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="13">
         <v>2756</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="14">
         <v>621.79999999999995</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="15">
         <v>50</v>
       </c>
-      <c r="I26" s="23">
+      <c r="I26" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="13">
         <v>2757</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="14">
         <v>1270.99</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="15">
         <v>50</v>
       </c>
-      <c r="I27" s="23">
+      <c r="I27" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="13">
         <v>2746</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="14">
         <v>1166.8956000000001</v>
       </c>
-      <c r="H28" s="22">
+      <c r="H28" s="15">
         <v>50</v>
       </c>
-      <c r="I28" s="23">
+      <c r="I28" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="13">
         <v>2756</v>
       </c>
-      <c r="G29" s="21">
+      <c r="G29" s="14">
         <v>1194.0989999999999</v>
       </c>
-      <c r="H29" s="29">
+      <c r="H29" s="22">
         <v>50</v>
       </c>
-      <c r="I29" s="23">
+      <c r="I29" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="18">
         <v>2752</v>
       </c>
-      <c r="G30" s="26">
+      <c r="G30" s="19">
         <v>1713.6880000000001</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H30" s="20">
         <v>50</v>
       </c>
-      <c r="I30" s="28">
+      <c r="I30" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="8">
         <v>3506</v>
       </c>
-      <c r="G31" s="16">
+      <c r="G31" s="9">
         <v>1.704</v>
       </c>
-      <c r="H31" s="17">
+      <c r="H31" s="10">
         <v>50</v>
       </c>
-      <c r="I31" s="18">
+      <c r="I31" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="20">
+      <c r="F32" s="13">
         <v>3134</v>
       </c>
-      <c r="G32" s="21">
+      <c r="G32" s="14">
         <v>747.59</v>
       </c>
-      <c r="H32" s="22">
+      <c r="H32" s="15">
         <v>50</v>
       </c>
-      <c r="I32" s="23">
+      <c r="I32" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="20">
+      <c r="F33" s="13">
         <v>3115</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G33" s="14">
         <v>1530.8</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H33" s="15">
         <v>50</v>
       </c>
-      <c r="I33" s="23">
+      <c r="I33" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="20">
+      <c r="F34" s="13">
         <v>3123</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="14">
         <v>1466.41</v>
       </c>
-      <c r="H34" s="22">
+      <c r="H34" s="15">
         <v>50</v>
       </c>
-      <c r="I34" s="23">
+      <c r="I34" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="13">
         <v>3128</v>
       </c>
-      <c r="G35" s="21">
+      <c r="G35" s="14">
         <v>1508.8</v>
       </c>
-      <c r="H35" s="29">
+      <c r="H35" s="22">
         <v>50</v>
       </c>
-      <c r="I35" s="23">
+      <c r="I35" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="25">
+      <c r="F36" s="18">
         <v>3114</v>
       </c>
-      <c r="G36" s="26">
+      <c r="G36" s="19">
         <v>2194.777</v>
       </c>
-      <c r="H36" s="27">
+      <c r="H36" s="20">
         <v>50</v>
       </c>
-      <c r="I36" s="28">
+      <c r="I36" s="21">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="15">
+      <c r="F37" s="8">
         <v>4435</v>
       </c>
-      <c r="G37" s="16">
+      <c r="G37" s="9">
         <v>4.0019999999999998</v>
       </c>
-      <c r="H37" s="17">
+      <c r="H37" s="10">
         <v>50</v>
       </c>
-      <c r="I37" s="18">
+      <c r="I37" s="11">
         <v>20</v>
       </c>
     </row>
     <row r="38" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="20">
+      <c r="F38" s="13">
         <v>3956</v>
       </c>
-      <c r="G38" s="21">
+      <c r="G38" s="14">
         <v>2327.1482999999998</v>
       </c>
-      <c r="H38" s="22">
+      <c r="H38" s="15">
         <v>50</v>
       </c>
-      <c r="I38" s="23">
+      <c r="I38" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="20">
+      <c r="F39" s="13">
         <v>3935</v>
       </c>
-      <c r="G39" s="21">
+      <c r="G39" s="14">
         <v>4675.1629999999996</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="15">
         <v>50</v>
       </c>
-      <c r="I39" s="23">
+      <c r="I39" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="20">
+      <c r="F40" s="13">
         <v>3937</v>
       </c>
-      <c r="G40" s="21">
+      <c r="G40" s="14">
         <v>4512.53</v>
       </c>
-      <c r="H40" s="22">
+      <c r="H40" s="15">
         <v>50</v>
       </c>
-      <c r="I40" s="23">
+      <c r="I40" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="20">
+      <c r="F41" s="13">
         <v>3950</v>
       </c>
-      <c r="G41" s="21">
+      <c r="G41" s="14">
         <v>4636.88</v>
       </c>
-      <c r="H41" s="29">
+      <c r="H41" s="22">
         <v>50</v>
       </c>
-      <c r="I41" s="23">
+      <c r="I41" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="42" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="25">
+      <c r="F42" s="18">
         <v>3913</v>
       </c>
-      <c r="G42" s="26">
+      <c r="G42" s="19">
         <v>6803.9</v>
       </c>
-      <c r="H42" s="27">
+      <c r="H42" s="20">
         <v>50</v>
       </c>
-      <c r="I42" s="28">
+      <c r="I42" s="21">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F43" s="15">
+      <c r="F43" s="8">
         <v>5563</v>
       </c>
-      <c r="G43" s="16">
+      <c r="G43" s="9">
         <v>3.1</v>
       </c>
-      <c r="H43" s="17">
+      <c r="H43" s="10">
         <v>100</v>
       </c>
-      <c r="I43" s="18">
+      <c r="I43" s="11">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="19" t="s">
+      <c r="E44" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="20">
+      <c r="F44" s="13">
         <v>5272</v>
       </c>
-      <c r="G44" s="21">
+      <c r="G44" s="14">
         <v>3530.2</v>
       </c>
-      <c r="H44" s="22">
+      <c r="H44" s="15">
         <v>100</v>
       </c>
-      <c r="I44" s="23">
+      <c r="I44" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="20">
+      <c r="F45" s="13">
         <v>5270</v>
       </c>
-      <c r="G45" s="21">
+      <c r="G45" s="14">
         <v>7075.23</v>
       </c>
-      <c r="H45" s="22">
+      <c r="H45" s="15">
         <v>100</v>
       </c>
-      <c r="I45" s="23">
+      <c r="I45" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E46" s="19" t="s">
+      <c r="E46" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="20">
+      <c r="F46" s="13">
         <v>5267</v>
       </c>
-      <c r="G46" s="21">
+      <c r="G46" s="14">
         <v>6550.08</v>
       </c>
-      <c r="H46" s="22">
+      <c r="H46" s="15">
         <v>100</v>
       </c>
-      <c r="I46" s="23">
+      <c r="I46" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E47" s="19" t="s">
+      <c r="E47" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F47" s="20">
+      <c r="F47" s="13">
         <v>5268</v>
       </c>
-      <c r="G47" s="21">
+      <c r="G47" s="14">
         <v>6802.027</v>
       </c>
-      <c r="H47" s="29">
+      <c r="H47" s="22">
         <v>100</v>
       </c>
-      <c r="I47" s="23">
+      <c r="I47" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E48" s="24" t="s">
+      <c r="E48" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F48" s="25">
+      <c r="F48" s="18">
         <v>5268</v>
       </c>
-      <c r="G48" s="26">
+      <c r="G48" s="19">
         <v>10161.31</v>
       </c>
-      <c r="H48" s="27">
+      <c r="H48" s="20">
         <v>100</v>
       </c>
-      <c r="I48" s="28">
+      <c r="I48" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E49" s="14" t="s">
+      <c r="E49" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F49" s="15">
+      <c r="F49" s="8">
         <v>11632</v>
       </c>
-      <c r="G49" s="16">
+      <c r="G49" s="9">
         <v>14.004</v>
       </c>
-      <c r="H49" s="17">
+      <c r="H49" s="10">
         <v>200</v>
       </c>
-      <c r="I49" s="18">
+      <c r="I49" s="11">
         <v>5</v>
       </c>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F50" s="20">
+      <c r="F50" s="13">
         <v>10942</v>
       </c>
-      <c r="G50" s="21">
+      <c r="G50" s="14">
         <v>84377</v>
       </c>
-      <c r="H50" s="22">
+      <c r="H50" s="15">
         <v>200</v>
       </c>
-      <c r="I50" s="23">
+      <c r="I50" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="51" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E51" s="19" t="s">
+      <c r="E51" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F51" s="20">
+      <c r="F51" s="13">
         <v>10942</v>
       </c>
-      <c r="G51" s="21">
+      <c r="G51" s="14">
         <v>142697.79999999999</v>
       </c>
-      <c r="H51" s="22">
+      <c r="H51" s="15">
         <v>200</v>
       </c>
-      <c r="I51" s="23">
+      <c r="I51" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="52" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E52" s="19" t="s">
+      <c r="E52" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="20">
+      <c r="F52" s="13">
         <v>10992</v>
       </c>
-      <c r="G52" s="21">
+      <c r="G52" s="14">
         <v>97108</v>
       </c>
-      <c r="H52" s="22">
+      <c r="H52" s="15">
         <v>200</v>
       </c>
-      <c r="I52" s="23">
+      <c r="I52" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="53" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E53" s="19" t="s">
+      <c r="E53" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F53" s="20">
+      <c r="F53" s="13">
         <v>10946</v>
       </c>
-      <c r="G53" s="21">
+      <c r="G53" s="14">
         <v>100799</v>
       </c>
-      <c r="H53" s="29">
+      <c r="H53" s="22">
         <v>200</v>
       </c>
-      <c r="I53" s="23">
+      <c r="I53" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="54" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E54" s="24" t="s">
+      <c r="E54" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="25">
+      <c r="F54" s="18">
         <v>10936</v>
       </c>
-      <c r="G54" s="26">
+      <c r="G54" s="19">
         <v>145707</v>
       </c>
-      <c r="H54" s="27">
+      <c r="H54" s="20">
         <v>200</v>
       </c>
-      <c r="I54" s="28">
+      <c r="I54" s="21">
         <v>5</v>
       </c>
+    </row>
+    <row r="55" spans="5:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E55" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="18">
+        <v>2297</v>
+      </c>
+      <c r="G55" s="19">
+        <v>953.4</v>
+      </c>
+      <c r="H55" s="20">
+        <v>20</v>
+      </c>
+      <c r="I55" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="5:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E56" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="18">
+        <v>2307</v>
+      </c>
+      <c r="G56" s="19">
+        <v>588.6</v>
+      </c>
+      <c r="H56" s="20">
+        <v>20</v>
+      </c>
+      <c r="I56" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="5:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E57" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="18">
+        <v>2326</v>
+      </c>
+      <c r="G57" s="19">
+        <v>356.8</v>
+      </c>
+      <c r="H57" s="20">
+        <v>20</v>
+      </c>
+      <c r="I57" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="5:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E58" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="18">
+        <v>3925</v>
+      </c>
+      <c r="G58" s="19">
+        <v>10703</v>
+      </c>
+      <c r="H58" s="20">
+        <v>50</v>
+      </c>
+      <c r="I58" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="5:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E59" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="18">
+        <v>4018</v>
+      </c>
+      <c r="G59" s="19">
+        <v>3839</v>
+      </c>
+      <c r="H59" s="20">
+        <v>50</v>
+      </c>
+      <c r="I59" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="5:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E60" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F60" s="18">
+        <v>1556</v>
+      </c>
+      <c r="G60" s="19">
+        <v>1765</v>
+      </c>
+      <c r="H60" s="20">
+        <v>20</v>
+      </c>
+      <c r="I60" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="5:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E61" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="18">
+        <v>11005</v>
+      </c>
+      <c r="G61" s="19">
+        <v>19008</v>
+      </c>
+      <c r="H61" s="20">
+        <v>200</v>
+      </c>
+      <c r="I61" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E62" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" s="18">
+        <v>10942</v>
+      </c>
+      <c r="G62" s="19">
+        <v>46945</v>
+      </c>
+      <c r="H62" s="20">
+        <v>200</v>
+      </c>
+      <c r="I62" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F7:F12">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5280,7 +5099,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13:F18">
-    <cfRule type="dataBar" priority="16">
+    <cfRule type="dataBar" priority="32">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5294,7 +5113,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:F24">
-    <cfRule type="dataBar" priority="15">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5308,7 +5127,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:F30">
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5322,7 +5141,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:F36">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5336,7 +5155,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37:F42">
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5350,7 +5169,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:F48">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5364,7 +5183,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:F54">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5378,7 +5197,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G12">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5392,7 +5211,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:G18">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5406,7 +5225,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G24">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5420,7 +5239,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25:G30">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5434,7 +5253,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:G36">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5448,7 +5267,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:G42">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5462,7 +5281,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G48">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5476,6 +5295,230 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49:G54">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3879161C-03D8-4C93-973E-595FAC9F211B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F55:F61">
+    <cfRule type="dataBar" priority="16">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7891F45B-A6D6-4D1D-AE5E-74553B11BE6A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G55:G61">
+    <cfRule type="dataBar" priority="15">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{58E7DE6E-EA1C-4E19-98E8-3D12E9F273E6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F56:F57">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1B3E2AA9-39C8-4DA5-A4B7-4511988F5EE7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56:G57">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{488DBB46-6A5C-423F-B1C3-F622461D5154}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F58">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BD03F405-424F-4CE7-83BE-E3D6DB329D01}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E5945905-9334-443D-994A-6D8C732FC5C2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F59">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BA4B1F59-49C7-4F38-91A9-81468C61A008}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G59">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{966E745F-CF07-40FC-87E3-447836D94594}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F60">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6C7959B4-6974-4564-9524-19BA5CDADE77}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G60">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F2740FFE-51C0-4FF1-8114-C5340074B262}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F61">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E2F78212-34A2-4C1A-8BC6-B2A49D1FF491}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G61">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F294BA35-9FB5-43A3-9409-487D26B5E94E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F62">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B4185349-29B2-44D0-98E4-8C0EDFB3B5CB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G62">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CD4A9BBC-CBF8-432F-BFDC-4D4D6A8BF7EF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F62">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DB5863A2-84D4-46D1-8620-8A9DED7CC691}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G62">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -5484,7 +5527,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3879161C-03D8-4C93-973E-595FAC9F211B}</x14:id>
+          <x14:id>{CE98F88F-8DF0-49D7-90FE-1B5B1A278624}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5686,8 +5729,337 @@
           </x14:cfRule>
           <xm:sqref>G49:G54</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7891F45B-A6D6-4D1D-AE5E-74553B11BE6A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F55:F61</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{58E7DE6E-EA1C-4E19-98E8-3D12E9F273E6}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G55:G61</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1B3E2AA9-39C8-4DA5-A4B7-4511988F5EE7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F56:F57</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{488DBB46-6A5C-423F-B1C3-F622461D5154}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G56:G57</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BD03F405-424F-4CE7-83BE-E3D6DB329D01}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F58</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E5945905-9334-443D-994A-6D8C732FC5C2}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G58</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BA4B1F59-49C7-4F38-91A9-81468C61A008}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F59</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{966E745F-CF07-40FC-87E3-447836D94594}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G59</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6C7959B4-6974-4564-9524-19BA5CDADE77}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F60</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F2740FFE-51C0-4FF1-8114-C5340074B262}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G60</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E2F78212-34A2-4C1A-8BC6-B2A49D1FF491}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F61</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F294BA35-9FB5-43A3-9409-487D26B5E94E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G61</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B4185349-29B2-44D0-98E4-8C0EDFB3B5CB}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F62</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CD4A9BBC-CBF8-432F-BFDC-4D4D6A8BF7EF}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G62</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DB5863A2-84D4-46D1-8620-8A9DED7CC691}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F62</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CE98F88F-8DF0-49D7-90FE-1B5B1A278624}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G62</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7376BE-C64E-4BF5-9D33-B914886586CB}">
+  <dimension ref="B1:C21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.5703125" style="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="35"/>
+      <c r="C3" s="28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B4" s="35"/>
+      <c r="C4" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="36"/>
+      <c r="C5" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" s="36"/>
+      <c r="C7" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
+      <c r="C9" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="36"/>
+      <c r="C10" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>